<commit_message>
Added some fixes for Program.cs and excel tusks inspect runner
</commit_message>
<xml_diff>
--- a/EpamTasksDirectories/DirectoriesInspectOutput.xlsx
+++ b/EpamTasksDirectories/DirectoriesInspectOutput.xlsx
@@ -36,7 +36,7 @@
     <t>13</t>
   </si>
   <si>
-    <t>00:00:00.044</t>
+    <t>00:00:00.042</t>
   </si>
   <si>
     <t xml:space="preserve">Duplicates: </t>
@@ -54,7 +54,7 @@
     <t>yhhh.txt</t>
   </si>
   <si>
-    <t>00:00:00.252</t>
+    <t>00:00:00.244</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated excel inspector with using OneDrive
</commit_message>
<xml_diff>
--- a/EpamTasksDirectories/DirectoriesInspectOutput.xlsx
+++ b/EpamTasksDirectories/DirectoriesInspectOutput.xlsx
@@ -36,7 +36,7 @@
     <t>13</t>
   </si>
   <si>
-    <t>00:00:00.042</t>
+    <t>00:00:00.048</t>
   </si>
   <si>
     <t xml:space="preserve">Duplicates: </t>
@@ -54,7 +54,7 @@
     <t>yhhh.txt</t>
   </si>
   <si>
-    <t>00:00:00.244</t>
+    <t>00:00:00.255</t>
   </si>
 </sst>
 </file>

</xml_diff>